<commit_message>
Add system design document
</commit_message>
<xml_diff>
--- a/doc/backend/db/TRN-MiniBlog_DatabaseDesign_TuanNguyen.xlsx
+++ b/doc/backend/db/TRN-MiniBlog_DatabaseDesign_TuanNguyen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="25605" windowHeight="14085" tabRatio="818" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="25605" windowHeight="14085" tabRatio="818" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -87,12 +87,12 @@
     <definedName name="項番3" localSheetId="7">#REF!</definedName>
     <definedName name="項番3">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="185">
   <si>
     <t>No</t>
   </si>
@@ -502,12 +502,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
     <t>Mini Blog</t>
   </si>
   <si>
@@ -526,9 +520,6 @@
     <t>image</t>
   </si>
   <si>
-    <t>intro</t>
-  </si>
-  <si>
     <t>Post Content</t>
   </si>
   <si>
@@ -538,15 +529,6 @@
     <t>TEXT</t>
   </si>
   <si>
-    <t>created_date</t>
-  </si>
-  <si>
-    <t>Active Status</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
     <t>BOOLEAN</t>
   </si>
   <si>
@@ -559,21 +541,9 @@
     <t>fk_posts_users</t>
   </si>
   <si>
-    <t>users_id</t>
-  </si>
-  <si>
     <t>Comment ID</t>
   </si>
   <si>
-    <t>posts_id</t>
-  </si>
-  <si>
-    <t>User post ID</t>
-  </si>
-  <si>
-    <t>posts_users_id</t>
-  </si>
-  <si>
     <t>Comment content</t>
   </si>
   <si>
@@ -586,9 +556,6 @@
     <t>tuanna</t>
   </si>
   <si>
-    <t xml:space="preserve">phone </t>
-  </si>
-  <si>
     <t>anh.tuan@mulodo.com</t>
   </si>
   <si>
@@ -613,9 +580,6 @@
     <t>image/iphone6.jpg</t>
   </si>
   <si>
-    <t>Iphone 6 …</t>
-  </si>
-  <si>
     <t>Video và hình ảnh chụp dưới nước bằng Samsung Galaxy S6 Active</t>
   </si>
   <si>
@@ -628,9 +592,6 @@
     <t>Apple vừa ….</t>
   </si>
   <si>
-    <t>Post introduction</t>
-  </si>
-  <si>
     <t>Hello</t>
   </si>
   <si>
@@ -641,6 +602,54 @@
   </si>
   <si>
     <t>fk_comments_posts1</t>
+  </si>
+  <si>
+    <t>Created time</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>Modified time</t>
+  </si>
+  <si>
+    <t>modified_at</t>
+  </si>
+  <si>
+    <t>Last login time</t>
+  </si>
+  <si>
+    <t>last_login</t>
+  </si>
+  <si>
+    <t>Login bash</t>
+  </si>
+  <si>
+    <t>login_bash</t>
+  </si>
+  <si>
+    <t>08/31/2015</t>
+  </si>
+  <si>
+    <t>author_id</t>
+  </si>
+  <si>
+    <t>Author ID</t>
+  </si>
+  <si>
+    <t>post_id</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Update fields</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
   </si>
 </sst>
 </file>
@@ -651,7 +660,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -832,19 +841,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF34495E"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -3039,7 +3035,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3406,24 +3402,34 @@
     <xf numFmtId="49" fontId="14" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="39" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3455,6 +3461,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3503,15 +3512,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3540,18 +3549,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5247,29 +5244,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="142"/>
-      <c r="P13" s="142"/>
-      <c r="Q13" s="142"/>
-      <c r="R13" s="142"/>
-      <c r="S13" s="142"/>
-      <c r="T13" s="142"/>
-      <c r="U13" s="142"/>
-      <c r="V13" s="142"/>
-      <c r="W13" s="142"/>
-      <c r="X13" s="142"/>
-      <c r="Y13" s="142"/>
-      <c r="Z13" s="142"/>
-      <c r="AA13" s="142"/>
-      <c r="AB13" s="142"/>
-      <c r="AC13" s="142"/>
-      <c r="AD13" s="142"/>
-      <c r="AE13" s="142"/>
-      <c r="AF13" s="142"/>
-      <c r="AG13" s="142"/>
-      <c r="AH13" s="142"/>
-      <c r="AI13" s="142"/>
-      <c r="AJ13" s="142"/>
-      <c r="AK13" s="142"/>
+      <c r="O13" s="146"/>
+      <c r="P13" s="146"/>
+      <c r="Q13" s="146"/>
+      <c r="R13" s="146"/>
+      <c r="S13" s="146"/>
+      <c r="T13" s="146"/>
+      <c r="U13" s="146"/>
+      <c r="V13" s="146"/>
+      <c r="W13" s="146"/>
+      <c r="X13" s="146"/>
+      <c r="Y13" s="146"/>
+      <c r="Z13" s="146"/>
+      <c r="AA13" s="146"/>
+      <c r="AB13" s="146"/>
+      <c r="AC13" s="146"/>
+      <c r="AD13" s="146"/>
+      <c r="AE13" s="146"/>
+      <c r="AF13" s="146"/>
+      <c r="AG13" s="146"/>
+      <c r="AH13" s="146"/>
+      <c r="AI13" s="146"/>
+      <c r="AJ13" s="146"/>
+      <c r="AK13" s="146"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -5301,29 +5298,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="142"/>
-      <c r="P14" s="142"/>
-      <c r="Q14" s="142"/>
-      <c r="R14" s="142"/>
-      <c r="S14" s="142"/>
-      <c r="T14" s="142"/>
-      <c r="U14" s="142"/>
-      <c r="V14" s="142"/>
-      <c r="W14" s="142"/>
-      <c r="X14" s="142"/>
-      <c r="Y14" s="142"/>
-      <c r="Z14" s="142"/>
-      <c r="AA14" s="142"/>
-      <c r="AB14" s="142"/>
-      <c r="AC14" s="142"/>
-      <c r="AD14" s="142"/>
-      <c r="AE14" s="142"/>
-      <c r="AF14" s="142"/>
-      <c r="AG14" s="142"/>
-      <c r="AH14" s="142"/>
-      <c r="AI14" s="142"/>
-      <c r="AJ14" s="142"/>
-      <c r="AK14" s="142"/>
+      <c r="O14" s="146"/>
+      <c r="P14" s="146"/>
+      <c r="Q14" s="146"/>
+      <c r="R14" s="146"/>
+      <c r="S14" s="146"/>
+      <c r="T14" s="146"/>
+      <c r="U14" s="146"/>
+      <c r="V14" s="146"/>
+      <c r="W14" s="146"/>
+      <c r="X14" s="146"/>
+      <c r="Y14" s="146"/>
+      <c r="Z14" s="146"/>
+      <c r="AA14" s="146"/>
+      <c r="AB14" s="146"/>
+      <c r="AC14" s="146"/>
+      <c r="AD14" s="146"/>
+      <c r="AE14" s="146"/>
+      <c r="AF14" s="146"/>
+      <c r="AG14" s="146"/>
+      <c r="AH14" s="146"/>
+      <c r="AI14" s="146"/>
+      <c r="AJ14" s="146"/>
+      <c r="AK14" s="146"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -5351,43 +5348,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="143" t="s">
+      <c r="K15" s="147" t="s">
         <v>112</v>
       </c>
-      <c r="L15" s="143"/>
-      <c r="M15" s="143"/>
-      <c r="N15" s="143"/>
-      <c r="O15" s="143"/>
-      <c r="P15" s="143"/>
-      <c r="Q15" s="143"/>
-      <c r="R15" s="143"/>
-      <c r="S15" s="143"/>
-      <c r="T15" s="143"/>
-      <c r="U15" s="143"/>
-      <c r="V15" s="143"/>
-      <c r="W15" s="143"/>
-      <c r="X15" s="143"/>
-      <c r="Y15" s="143"/>
-      <c r="Z15" s="143"/>
-      <c r="AA15" s="143"/>
-      <c r="AB15" s="143"/>
-      <c r="AC15" s="143"/>
-      <c r="AD15" s="143"/>
-      <c r="AE15" s="143"/>
-      <c r="AF15" s="143"/>
-      <c r="AG15" s="143"/>
-      <c r="AH15" s="143"/>
-      <c r="AI15" s="143"/>
-      <c r="AJ15" s="143"/>
-      <c r="AK15" s="143"/>
-      <c r="AL15" s="143"/>
-      <c r="AM15" s="143"/>
-      <c r="AN15" s="143"/>
-      <c r="AO15" s="143"/>
-      <c r="AP15" s="143"/>
-      <c r="AQ15" s="143"/>
-      <c r="AR15" s="143"/>
-      <c r="AS15" s="143"/>
+      <c r="L15" s="147"/>
+      <c r="M15" s="147"/>
+      <c r="N15" s="147"/>
+      <c r="O15" s="147"/>
+      <c r="P15" s="147"/>
+      <c r="Q15" s="147"/>
+      <c r="R15" s="147"/>
+      <c r="S15" s="147"/>
+      <c r="T15" s="147"/>
+      <c r="U15" s="147"/>
+      <c r="V15" s="147"/>
+      <c r="W15" s="147"/>
+      <c r="X15" s="147"/>
+      <c r="Y15" s="147"/>
+      <c r="Z15" s="147"/>
+      <c r="AA15" s="147"/>
+      <c r="AB15" s="147"/>
+      <c r="AC15" s="147"/>
+      <c r="AD15" s="147"/>
+      <c r="AE15" s="147"/>
+      <c r="AF15" s="147"/>
+      <c r="AG15" s="147"/>
+      <c r="AH15" s="147"/>
+      <c r="AI15" s="147"/>
+      <c r="AJ15" s="147"/>
+      <c r="AK15" s="147"/>
+      <c r="AL15" s="147"/>
+      <c r="AM15" s="147"/>
+      <c r="AN15" s="147"/>
+      <c r="AO15" s="147"/>
+      <c r="AP15" s="147"/>
+      <c r="AQ15" s="147"/>
+      <c r="AR15" s="147"/>
+      <c r="AS15" s="147"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -5407,41 +5404,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="143"/>
-      <c r="L16" s="143"/>
-      <c r="M16" s="143"/>
-      <c r="N16" s="143"/>
-      <c r="O16" s="143"/>
-      <c r="P16" s="143"/>
-      <c r="Q16" s="143"/>
-      <c r="R16" s="143"/>
-      <c r="S16" s="143"/>
-      <c r="T16" s="143"/>
-      <c r="U16" s="143"/>
-      <c r="V16" s="143"/>
-      <c r="W16" s="143"/>
-      <c r="X16" s="143"/>
-      <c r="Y16" s="143"/>
-      <c r="Z16" s="143"/>
-      <c r="AA16" s="143"/>
-      <c r="AB16" s="143"/>
-      <c r="AC16" s="143"/>
-      <c r="AD16" s="143"/>
-      <c r="AE16" s="143"/>
-      <c r="AF16" s="143"/>
-      <c r="AG16" s="143"/>
-      <c r="AH16" s="143"/>
-      <c r="AI16" s="143"/>
-      <c r="AJ16" s="143"/>
-      <c r="AK16" s="143"/>
-      <c r="AL16" s="143"/>
-      <c r="AM16" s="143"/>
-      <c r="AN16" s="143"/>
-      <c r="AO16" s="143"/>
-      <c r="AP16" s="143"/>
-      <c r="AQ16" s="143"/>
-      <c r="AR16" s="143"/>
-      <c r="AS16" s="143"/>
+      <c r="K16" s="147"/>
+      <c r="L16" s="147"/>
+      <c r="M16" s="147"/>
+      <c r="N16" s="147"/>
+      <c r="O16" s="147"/>
+      <c r="P16" s="147"/>
+      <c r="Q16" s="147"/>
+      <c r="R16" s="147"/>
+      <c r="S16" s="147"/>
+      <c r="T16" s="147"/>
+      <c r="U16" s="147"/>
+      <c r="V16" s="147"/>
+      <c r="W16" s="147"/>
+      <c r="X16" s="147"/>
+      <c r="Y16" s="147"/>
+      <c r="Z16" s="147"/>
+      <c r="AA16" s="147"/>
+      <c r="AB16" s="147"/>
+      <c r="AC16" s="147"/>
+      <c r="AD16" s="147"/>
+      <c r="AE16" s="147"/>
+      <c r="AF16" s="147"/>
+      <c r="AG16" s="147"/>
+      <c r="AH16" s="147"/>
+      <c r="AI16" s="147"/>
+      <c r="AJ16" s="147"/>
+      <c r="AK16" s="147"/>
+      <c r="AL16" s="147"/>
+      <c r="AM16" s="147"/>
+      <c r="AN16" s="147"/>
+      <c r="AO16" s="147"/>
+      <c r="AP16" s="147"/>
+      <c r="AQ16" s="147"/>
+      <c r="AR16" s="147"/>
+      <c r="AS16" s="147"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6030,14 +6027,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="144" t="s">
+      <c r="AN27" s="148" t="s">
         <v>114</v>
       </c>
-      <c r="AO27" s="144"/>
-      <c r="AP27" s="144"/>
-      <c r="AQ27" s="144"/>
-      <c r="AR27" s="144"/>
-      <c r="AS27" s="144"/>
+      <c r="AO27" s="148"/>
+      <c r="AP27" s="148"/>
+      <c r="AQ27" s="148"/>
+      <c r="AR27" s="148"/>
+      <c r="AS27" s="148"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -6496,7 +6493,7 @@
   <dimension ref="B1:F34"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -6546,10 +6543,18 @@
       <c r="F3" s="96"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="97"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="99"/>
+      <c r="B4" s="142" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="143" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="144" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="145" t="s">
+        <v>183</v>
+      </c>
       <c r="F4" s="100"/>
     </row>
     <row r="5" spans="2:6">
@@ -6788,11 +6793,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" thickBot="1">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="149" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
     </row>
     <row r="2" spans="1:3" ht="12.75" thickBot="1">
       <c r="A2" s="118" t="s">
@@ -7046,10 +7051,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="I10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -7065,10 +7070,11 @@
     <col min="12" max="12" width="12.7109375" style="13" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" style="13" customWidth="1"/>
     <col min="14" max="15" width="19.28515625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="17" style="137" customWidth="1"/>
+    <col min="16" max="16" width="17" style="136" customWidth="1"/>
     <col min="17" max="17" width="17" style="13" customWidth="1"/>
     <col min="18" max="18" width="15.42578125" style="13" customWidth="1"/>
-    <col min="19" max="16384" width="8.85546875" style="13"/>
+    <col min="19" max="19" width="15" style="13" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" thickBot="1">
@@ -7080,103 +7086,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="146" t="s">
+      <c r="C2" s="150" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="147"/>
+      <c r="D2" s="151"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="146" t="s">
+      <c r="F2" s="150" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="150"/>
+      <c r="G2" s="154"/>
     </row>
     <row r="3" spans="1:19" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="151" t="s">
+      <c r="F3" s="155" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="152"/>
+      <c r="G3" s="156"/>
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="152" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="149"/>
+      <c r="D4" s="153"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="148"/>
-      <c r="G4" s="152"/>
+      <c r="F4" s="157" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="156"/>
     </row>
     <row r="5" spans="1:19" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="149"/>
+      <c r="D5" s="153"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="156"/>
     </row>
     <row r="6" spans="1:19" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="152" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="149"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="152"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="156"/>
     </row>
     <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="159"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="160"/>
-      <c r="C8" s="161"/>
-      <c r="D8" s="161"/>
-      <c r="E8" s="161"/>
-      <c r="F8" s="161"/>
-      <c r="G8" s="162"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="163"/>
-      <c r="C9" s="161"/>
-      <c r="D9" s="161"/>
-      <c r="E9" s="161"/>
-      <c r="F9" s="161"/>
-      <c r="G9" s="162"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="164"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="165"/>
-      <c r="G10" s="166"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -7186,7 +7194,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" ht="24">
       <c r="A13" s="30" t="s">
         <v>0</v>
       </c>
@@ -7208,33 +7216,39 @@
       <c r="G13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="128" t="s">
+      <c r="I13" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="J13" s="128" t="s">
+      <c r="J13" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="K13" s="128" t="s">
+      <c r="K13" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="L13" s="128"/>
-      <c r="M13" s="128" t="s">
+      <c r="L13" s="31"/>
+      <c r="M13" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="N13" s="128" t="s">
+      <c r="N13" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="O13" s="128" t="s">
+      <c r="O13" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="P13" s="138" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q13" s="128"/>
-      <c r="R13" s="128"/>
-      <c r="S13" s="128"/>
-    </row>
-    <row r="14" spans="1:19" ht="15">
+      <c r="P13" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q13" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="R13" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="S13" s="31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="69">
         <v>1</v>
       </c>
@@ -7247,39 +7261,43 @@
       <c r="D14" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="66" t="s">
-        <v>3</v>
+      <c r="E14" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F14" s="67"/>
       <c r="G14" s="106" t="s">
         <v>50</v>
       </c>
       <c r="H14" s="87"/>
-      <c r="I14" s="13">
+      <c r="I14" s="69">
         <v>1</v>
       </c>
-      <c r="J14" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="K14" s="13" t="s">
+      <c r="J14" s="63" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="M14" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="N14" s="136" t="s">
-        <v>161</v>
-      </c>
-      <c r="O14" s="136" t="s">
-        <v>164</v>
-      </c>
-      <c r="P14" s="137">
-        <v>987890031</v>
-      </c>
-      <c r="Q14" s="127"/>
-      <c r="R14" s="127"/>
-    </row>
-    <row r="15" spans="1:19" ht="15">
+      <c r="L14" s="65"/>
+      <c r="M14" s="140" t="s">
+        <v>150</v>
+      </c>
+      <c r="N14" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="O14" s="106" t="s">
+        <v>153</v>
+      </c>
+      <c r="P14" s="69"/>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="64">
+        <v>1440992679</v>
+      </c>
+      <c r="S14" s="65">
+        <v>1440992958</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="59">
         <f>A14+1</f>
         <v>2</v>
@@ -7293,41 +7311,45 @@
       <c r="D15" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="E15" s="66" t="s">
-        <v>3</v>
+      <c r="E15" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F15" s="67"/>
       <c r="G15" s="107" t="s">
         <v>106</v>
       </c>
       <c r="H15" s="87"/>
-      <c r="I15" s="13">
+      <c r="I15" s="59">
         <v>2</v>
       </c>
-      <c r="J15" s="139" t="s">
-        <v>165</v>
-      </c>
-      <c r="K15" s="13" t="s">
+      <c r="J15" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="K15" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="M15" s="139" t="s">
-        <v>160</v>
-      </c>
-      <c r="N15" s="136" t="s">
-        <v>166</v>
-      </c>
-      <c r="O15" s="136" t="s">
-        <v>167</v>
-      </c>
-      <c r="P15" s="137">
-        <v>987481234</v>
-      </c>
-      <c r="Q15" s="127"/>
-      <c r="R15" s="127"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="140" t="s">
+        <v>150</v>
+      </c>
+      <c r="N15" s="67" t="s">
+        <v>155</v>
+      </c>
+      <c r="O15" s="107" t="s">
+        <v>156</v>
+      </c>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="65">
+        <v>1440992958</v>
+      </c>
+      <c r="S15" s="65">
+        <v>1440992988</v>
+      </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="59">
-        <f t="shared" ref="A16:A20" si="0">A15+1</f>
+        <f t="shared" ref="A16:A19" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
@@ -7339,8 +7361,8 @@
       <c r="D16" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="66" t="s">
-        <v>3</v>
+      <c r="E16" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
@@ -7362,8 +7384,8 @@
       <c r="D17" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="E17" s="66" t="s">
-        <v>3</v>
+      <c r="E17" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117"/>
@@ -7382,8 +7404,8 @@
       <c r="D18" s="129" t="s">
         <v>129</v>
       </c>
-      <c r="E18" s="66" t="s">
-        <v>3</v>
+      <c r="E18" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106"/>
@@ -7402,158 +7424,234 @@
       <c r="D19" s="129" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="66" t="s">
-        <v>3</v>
+      <c r="E19" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="59">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="D20" s="129" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="66" t="s">
-        <v>0</v>
+        <v>146</v>
+      </c>
+      <c r="E20" s="140" t="s">
+        <v>181</v>
       </c>
       <c r="F20" s="67"/>
       <c r="G20" s="106"/>
     </row>
-    <row r="22" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A22" s="1" t="s">
+    <row r="21" spans="1:7">
+      <c r="A21" s="59">
+        <v>8</v>
+      </c>
+      <c r="B21" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" s="129" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" s="140" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21" s="67"/>
+      <c r="G21" s="106"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="59">
+        <v>9</v>
+      </c>
+      <c r="B22" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="129" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="67"/>
+      <c r="G22" s="106"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="59">
+        <v>10</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="129" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="140" t="s">
+        <v>181</v>
+      </c>
+      <c r="F23" s="67"/>
+      <c r="G23" s="106"/>
+    </row>
+    <row r="24" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A24" s="56"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="174"/>
+      <c r="D24" s="175"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="55"/>
+    </row>
+    <row r="26" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="24">
-      <c r="A23" s="29" t="s">
+    <row r="27" spans="1:7" ht="24">
+      <c r="A27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="153" t="s">
+      <c r="C27" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="154"/>
-      <c r="E23" s="34" t="s">
+      <c r="D27" s="159"/>
+      <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="34" t="s">
+      <c r="F27" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="35" t="s">
+      <c r="G27" s="35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.25">
-      <c r="A24" s="14">
+    <row r="28" spans="1:7" ht="14.25">
+      <c r="A28" s="14">
         <v>1</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="167" t="s">
+      <c r="C28" s="172" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="168"/>
-      <c r="E24" s="46" t="s">
+      <c r="D28" s="173"/>
+      <c r="E28" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="46" t="s">
+      <c r="F28" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="20"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="57">
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="57">
         <v>2</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="172"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="53"/>
-    </row>
-    <row r="26" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A26" s="56">
+      <c r="B29" s="51" t="s">
+        <v>184</v>
+      </c>
+      <c r="C29" s="177" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="178"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="170"/>
-      <c r="D26" s="171"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="55"/>
-    </row>
-    <row r="28" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
-      <c r="A28" s="1" t="s">
+      <c r="G29" s="53"/>
+    </row>
+    <row r="30" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A30" s="56">
+        <v>3</v>
+      </c>
+      <c r="B30" s="54"/>
+      <c r="C30" s="174" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="175"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="55"/>
+    </row>
+    <row r="32" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
+      <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
-      <c r="A29" s="36" t="s">
+    <row r="33" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
+      <c r="A33" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="155" t="s">
+      <c r="C33" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="156"/>
-      <c r="E29" s="155" t="s">
+      <c r="D33" s="161"/>
+      <c r="E33" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="169"/>
-      <c r="G29" s="38" t="s">
+      <c r="F33" s="176"/>
+      <c r="G33" s="38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A31" s="1" t="s">
+    <row r="35" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" thickBot="1">
-      <c r="A32" s="36" t="s">
+    <row r="36" spans="1:7" ht="15" thickBot="1">
+      <c r="A36" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="155" t="s">
+      <c r="C36" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="156"/>
-      <c r="E32" s="155" t="s">
+      <c r="D36" s="161"/>
+      <c r="E36" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="169"/>
-      <c r="G32" s="38" t="s">
+      <c r="F36" s="176"/>
+      <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C23:D23"/>
+  <mergeCells count="21">
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C30:D30"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C33:D33"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -7582,10 +7680,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -7600,9 +7698,9 @@
     <col min="11" max="11" width="54" style="13" customWidth="1"/>
     <col min="12" max="12" width="17.85546875" style="13" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" style="13" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="137" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="136" customWidth="1"/>
     <col min="15" max="15" width="19.28515625" style="13" customWidth="1"/>
-    <col min="16" max="17" width="17" style="137" customWidth="1"/>
+    <col min="16" max="17" width="17" style="136" customWidth="1"/>
     <col min="18" max="18" width="15.42578125" style="13" customWidth="1"/>
     <col min="19" max="16384" width="8.85546875" style="13"/>
   </cols>
@@ -7616,103 +7714,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="146" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="147"/>
+      <c r="C2" s="150" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="151"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="146" t="s">
+      <c r="F2" s="150" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="150"/>
+      <c r="G2" s="154"/>
     </row>
     <row r="3" spans="1:19" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="151" t="s">
+      <c r="F3" s="155" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="152"/>
+      <c r="G3" s="156"/>
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="152" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="149"/>
+      <c r="D4" s="153"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="148"/>
-      <c r="G4" s="152"/>
+      <c r="F4" s="157" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="156"/>
     </row>
     <row r="5" spans="1:19" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="152" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="149"/>
+      <c r="D5" s="153"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="156"/>
     </row>
     <row r="6" spans="1:19" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="152" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="149"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="152"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="156"/>
     </row>
     <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="159"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="160"/>
-      <c r="C8" s="161"/>
-      <c r="D8" s="161"/>
-      <c r="E8" s="161"/>
-      <c r="F8" s="161"/>
-      <c r="G8" s="162"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="163"/>
-      <c r="C9" s="161"/>
-      <c r="D9" s="161"/>
-      <c r="E9" s="161"/>
-      <c r="F9" s="161"/>
-      <c r="G9" s="162"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="164"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="165"/>
-      <c r="G10" s="166"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -7744,31 +7844,28 @@
       <c r="G13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="128" t="s">
+      <c r="I13" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="J13" s="141" t="s">
-        <v>154</v>
-      </c>
-      <c r="K13" s="141" t="s">
+      <c r="J13" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="K13" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="L13" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="L13" s="141" t="s">
+      <c r="M13" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="M13" s="141" t="s">
-        <v>143</v>
-      </c>
-      <c r="N13" s="182" t="s">
-        <v>145</v>
-      </c>
-      <c r="O13" s="141" t="s">
-        <v>147</v>
-      </c>
-      <c r="P13" s="182" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q13" s="182" t="s">
+      <c r="N13" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="O13" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="P13" s="30" t="s">
         <v>6</v>
       </c>
       <c r="R13" s="128"/>
@@ -7779,7 +7876,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C14" s="64" t="s">
         <v>110</v>
@@ -7787,39 +7884,34 @@
       <c r="D14" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="66" t="s">
-        <v>3</v>
+      <c r="E14" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F14" s="67"/>
       <c r="G14" s="106" t="s">
         <v>50</v>
       </c>
       <c r="H14" s="87"/>
-      <c r="I14" s="13">
+      <c r="I14" s="69">
         <v>1</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="63">
         <v>1</v>
       </c>
-      <c r="K14" s="139" t="s">
-        <v>170</v>
-      </c>
-      <c r="L14" s="139" t="s">
-        <v>171</v>
-      </c>
-      <c r="M14" s="139" t="s">
-        <v>172</v>
-      </c>
-      <c r="N14" s="139" t="s">
-        <v>176</v>
-      </c>
-      <c r="O14" s="139">
+      <c r="K14" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="L14" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="M14" s="140" t="s">
+        <v>164</v>
+      </c>
+      <c r="N14" s="67">
         <v>1440496324</v>
       </c>
-      <c r="P14" s="137">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="137">
+      <c r="O14" s="106"/>
+      <c r="P14" s="69">
         <v>1</v>
       </c>
       <c r="R14" s="127"/>
@@ -7829,107 +7921,108 @@
         <f>A14+1</f>
         <v>2</v>
       </c>
-      <c r="B15" s="63" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="65" t="s">
-        <v>154</v>
+      <c r="B15" s="138" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="141" t="s">
+        <v>178</v>
       </c>
       <c r="D15" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="66" t="s">
-        <v>3</v>
+      <c r="E15" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F15" s="67"/>
       <c r="G15" s="107"/>
       <c r="H15" s="87"/>
-      <c r="I15" s="13">
+      <c r="I15" s="59">
         <v>2</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="138">
         <v>1</v>
       </c>
-      <c r="K15" s="139" t="s">
-        <v>173</v>
-      </c>
-      <c r="L15" s="139" t="s">
-        <v>174</v>
-      </c>
-      <c r="M15" s="139" t="s">
-        <v>175</v>
-      </c>
-      <c r="N15" s="139" t="s">
-        <v>175</v>
-      </c>
-      <c r="O15" s="139">
+      <c r="K15" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="L15" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="M15" s="140" t="s">
+        <v>163</v>
+      </c>
+      <c r="N15" s="67">
         <v>1440496324</v>
       </c>
-      <c r="P15" s="137">
+      <c r="O15" s="107"/>
+      <c r="P15" s="59">
         <v>1</v>
       </c>
-      <c r="Q15" s="137">
-        <v>1</v>
-      </c>
       <c r="R15" s="127"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="59">
-        <f t="shared" ref="A16:A20" si="0">A15+1</f>
+      <c r="A16" s="69">
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D16" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="66" t="s">
-        <v>3</v>
+      <c r="E16" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117"/>
       <c r="H16" s="87"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="140"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="117"/>
+      <c r="P16" s="69"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="59">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A17:A19" si="0">A16+1</f>
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D17" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="66" t="s">
-        <v>0</v>
+      <c r="E17" s="140" t="s">
+        <v>181</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="59">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B18" s="184" t="s">
-        <v>177</v>
+      <c r="B18" s="63" t="s">
+        <v>141</v>
       </c>
       <c r="C18" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="129" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="129" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="66" t="s">
-        <v>3</v>
+      <c r="E18" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106"/>
@@ -7939,759 +8032,187 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B19" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" s="65" t="s">
-        <v>145</v>
-      </c>
-      <c r="D19" s="129" t="s">
+      <c r="B19" s="138" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" s="141" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="E19" s="66" t="s">
-        <v>3</v>
+      <c r="E19" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="59">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B20" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="65" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="E20" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" s="67"/>
-      <c r="G20" s="106"/>
+      <c r="B20" s="138" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="141" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" s="141" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="140" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="137" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="59">
         <v>8</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>149</v>
+        <v>6</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="E21" s="66" t="s">
-        <v>3</v>
+        <v>144</v>
+      </c>
+      <c r="E21" s="140" t="s">
+        <v>1</v>
       </c>
       <c r="F21" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="140" t="s">
-        <v>168</v>
+      <c r="G21" s="137" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="59">
-        <v>9</v>
-      </c>
-      <c r="B22" s="63" t="s">
-        <v>151</v>
-      </c>
-      <c r="C22" s="65" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="E22" s="66" t="s">
+      <c r="A22" s="59"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="106"/>
+    </row>
+    <row r="23" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A23" s="70"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="135"/>
+      <c r="G23" s="134"/>
+    </row>
+    <row r="25" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="24">
+      <c r="A26" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="158" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="159"/>
+      <c r="E26" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14.25">
+      <c r="A27" s="14">
+        <v>1</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="172" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="173"/>
+      <c r="E27" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="67" t="s">
-        <v>98</v>
-      </c>
-      <c r="G22" s="140" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="59"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="106"/>
-    </row>
-    <row r="24" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A24" s="70"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="133"/>
-      <c r="F24" s="135"/>
-      <c r="G24" s="134"/>
-    </row>
-    <row r="26" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="24">
-      <c r="A27" s="29" t="s">
+      <c r="F27" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:7" ht="12.95" customHeight="1">
+      <c r="A28" s="57">
+        <v>2</v>
+      </c>
+      <c r="B28" s="51"/>
+      <c r="C28" s="177"/>
+      <c r="D28" s="178"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="53"/>
+    </row>
+    <row r="29" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
+      <c r="A29" s="56">
+        <v>3</v>
+      </c>
+      <c r="B29" s="54"/>
+      <c r="C29" s="174"/>
+      <c r="D29" s="175"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="55"/>
+    </row>
+    <row r="31" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" thickBot="1">
+      <c r="A32" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="153" t="s">
+      <c r="B32" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="154"/>
-      <c r="E27" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="14.25">
-      <c r="A28" s="14">
-        <v>1</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="167" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="168"/>
-      <c r="E28" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:7" ht="12.95" customHeight="1">
-      <c r="A29" s="57">
-        <v>2</v>
-      </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="172"/>
-      <c r="D29" s="173"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="53"/>
-    </row>
-    <row r="30" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
-      <c r="A30" s="56">
-        <v>3</v>
-      </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="170"/>
-      <c r="D30" s="171"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="55"/>
-    </row>
-    <row r="32" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A32" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1">
-      <c r="A33" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="155" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="156"/>
-      <c r="E33" s="155" t="s">
+      <c r="D32" s="161"/>
+      <c r="E32" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="169"/>
-      <c r="G33" s="38" t="s">
+      <c r="F32" s="176"/>
+      <c r="G32" s="38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
-      <c r="B34" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E34" s="18" t="s">
+    <row r="33" spans="1:7">
+      <c r="B33" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="139" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="G34" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A35" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15" thickBot="1">
-      <c r="A36" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="155" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="156"/>
-      <c r="E36" s="155" t="s">
-        <v>37</v>
-      </c>
-      <c r="F36" s="169"/>
-      <c r="G36" s="38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="18" customWidth="1"/>
-    <col min="3" max="4" width="14.7109375" style="18" customWidth="1"/>
-    <col min="5" max="6" width="10.140625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="18" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.85546875" style="13"/>
-    <col min="11" max="11" width="17.7109375" style="13" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="13" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="13" customWidth="1"/>
-    <col min="14" max="15" width="19.28515625" style="13" customWidth="1"/>
-    <col min="16" max="17" width="17" style="13" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="13" customWidth="1"/>
-    <col min="19" max="16384" width="8.85546875" style="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" ht="12.75" thickBot="1">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="14.25">
-      <c r="B2" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="146" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="147"/>
-      <c r="E2" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="146" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="150"/>
-    </row>
-    <row r="3" spans="1:19" ht="14.25">
-      <c r="B3" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149"/>
-      <c r="E3" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="151" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3" s="152"/>
-    </row>
-    <row r="4" spans="1:19" ht="14.25">
-      <c r="B4" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="148" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="149"/>
-      <c r="E4" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="148"/>
-      <c r="G4" s="152"/>
-    </row>
-    <row r="5" spans="1:19" ht="24">
-      <c r="B5" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="148" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="149"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="152"/>
-    </row>
-    <row r="6" spans="1:19" ht="24">
-      <c r="B6" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="148" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="149"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="152"/>
-    </row>
-    <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="157" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="159"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="B8" s="160"/>
-      <c r="C8" s="161"/>
-      <c r="D8" s="161"/>
-      <c r="E8" s="161"/>
-      <c r="F8" s="161"/>
-      <c r="G8" s="162"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="B9" s="163"/>
-      <c r="C9" s="161"/>
-      <c r="D9" s="161"/>
-      <c r="E9" s="161"/>
-      <c r="F9" s="161"/>
-      <c r="G9" s="162"/>
-    </row>
-    <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="164"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="165"/>
-      <c r="G10" s="166"/>
-    </row>
-    <row r="12" spans="1:19" ht="12.75" thickBot="1">
-      <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="128" t="s">
-        <v>110</v>
-      </c>
-      <c r="J13" s="141" t="s">
-        <v>154</v>
-      </c>
-      <c r="K13" s="141" t="s">
-        <v>156</v>
-      </c>
-      <c r="L13" s="141" t="s">
-        <v>158</v>
-      </c>
-      <c r="M13" s="141" t="s">
-        <v>145</v>
-      </c>
-      <c r="N13" s="141" t="s">
-        <v>147</v>
-      </c>
-      <c r="O13" s="128"/>
-      <c r="P13" s="128"/>
-      <c r="Q13" s="128"/>
-      <c r="R13" s="128"/>
-      <c r="S13" s="128"/>
-    </row>
-    <row r="14" spans="1:19" ht="15">
-      <c r="A14" s="69">
-        <v>1</v>
-      </c>
-      <c r="B14" s="63" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="67"/>
-      <c r="G14" s="106" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="87"/>
-      <c r="I14" s="13">
-        <v>1</v>
-      </c>
-      <c r="J14" s="13">
-        <v>1</v>
-      </c>
-      <c r="K14" s="13">
-        <v>1</v>
-      </c>
-      <c r="L14" s="13">
-        <v>1</v>
-      </c>
-      <c r="M14" s="139" t="s">
-        <v>178</v>
-      </c>
-      <c r="N14" s="183">
-        <v>1440496324</v>
-      </c>
-      <c r="P14" s="127"/>
-      <c r="Q14" s="127"/>
-      <c r="R14" s="127"/>
-    </row>
-    <row r="15" spans="1:19" ht="15">
-      <c r="A15" s="59">
-        <f>A14+1</f>
-        <v>2</v>
-      </c>
-      <c r="B15" s="63" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="65" t="s">
-        <v>154</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="67"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="13">
-        <v>2</v>
-      </c>
-      <c r="J15" s="13">
-        <v>2</v>
-      </c>
-      <c r="K15" s="13">
-        <v>1</v>
-      </c>
-      <c r="L15" s="13">
-        <v>1</v>
-      </c>
-      <c r="M15" s="139" t="s">
-        <v>179</v>
-      </c>
-      <c r="N15" s="183">
-        <v>1440496390</v>
-      </c>
-      <c r="P15" s="127"/>
-      <c r="Q15" s="127"/>
-      <c r="R15" s="127"/>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="59">
-        <f t="shared" ref="A16:A18" si="0">A15+1</f>
-        <v>3</v>
-      </c>
-      <c r="B16" s="63" t="s">
-        <v>138</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>156</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="67"/>
-      <c r="G16" s="117"/>
-      <c r="H16" s="87"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="59">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B17" s="63" t="s">
-        <v>157</v>
-      </c>
-      <c r="C17" s="65" t="s">
-        <v>158</v>
-      </c>
-      <c r="D17" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="117"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="59">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B18" s="63" t="s">
-        <v>159</v>
-      </c>
-      <c r="C18" s="65" t="s">
-        <v>145</v>
-      </c>
-      <c r="D18" s="65" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="67"/>
-      <c r="G18" s="106"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="59">
-        <v>6</v>
-      </c>
-      <c r="B19" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="65" t="s">
-        <v>147</v>
-      </c>
-      <c r="D19" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="E19" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" s="67"/>
-      <c r="G19" s="106"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="59"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="106"/>
-    </row>
-    <row r="21" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A21" s="70"/>
-      <c r="B21" s="131"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="132"/>
-      <c r="E21" s="133"/>
-      <c r="F21" s="135"/>
-      <c r="G21" s="134"/>
-    </row>
-    <row r="23" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A23" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="24">
-      <c r="A24" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="153" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="154"/>
-      <c r="E24" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="14.25">
-      <c r="A25" s="14">
-        <v>1</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="167" t="s">
-        <v>110</v>
-      </c>
-      <c r="D25" s="168"/>
-      <c r="E25" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="20"/>
-    </row>
-    <row r="26" spans="1:7" ht="12.95" customHeight="1">
-      <c r="A26" s="57">
-        <v>2</v>
-      </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="172"/>
-      <c r="D26" s="173"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="53"/>
-    </row>
-    <row r="27" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
-      <c r="A27" s="56">
-        <v>3</v>
-      </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="170"/>
-      <c r="D27" s="171"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="55"/>
-    </row>
-    <row r="29" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A29" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15" thickBot="1">
-      <c r="A30" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="155" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="156"/>
-      <c r="E30" s="155" t="s">
-        <v>36</v>
-      </c>
-      <c r="F30" s="169"/>
-      <c r="G30" s="38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="B31" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="B32" s="185" t="s">
-        <v>181</v>
-      </c>
-      <c r="C32" s="185" t="s">
-        <v>156</v>
-      </c>
-      <c r="E32" s="185" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="185" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="C33" s="185" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" s="185" t="s">
-        <v>119</v>
-      </c>
-      <c r="G33" s="185" t="s">
+      <c r="G33" s="18" t="s">
         <v>110</v>
       </c>
     </row>
@@ -8707,14 +8228,14 @@
       <c r="B35" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="155" t="s">
+      <c r="C35" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="156"/>
-      <c r="E35" s="155" t="s">
+      <c r="D35" s="161"/>
+      <c r="E35" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="169"/>
+      <c r="F35" s="176"/>
       <c r="G35" s="38" t="s">
         <v>39</v>
       </c>
@@ -8735,12 +8256,539 @@
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="18" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" style="18" customWidth="1"/>
+    <col min="5" max="6" width="10.140625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" style="18" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.85546875" style="13"/>
+    <col min="11" max="11" width="17.7109375" style="13" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="13" customWidth="1"/>
+    <col min="13" max="15" width="19.28515625" style="13" customWidth="1"/>
+    <col min="16" max="17" width="17" style="13" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="13" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="12.75" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="14.25">
+      <c r="B2" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="150" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="151"/>
+      <c r="E2" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="150" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="154"/>
+    </row>
+    <row r="3" spans="1:19" ht="14.25">
+      <c r="B3" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="155" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="156"/>
+    </row>
+    <row r="4" spans="1:19" ht="14.25">
+      <c r="B4" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="152" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="153"/>
+      <c r="E4" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="157" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="156"/>
+    </row>
+    <row r="5" spans="1:19" ht="24">
+      <c r="B5" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="152" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="153"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="156"/>
+    </row>
+    <row r="6" spans="1:19" ht="24">
+      <c r="B6" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="152" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="153"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="156"/>
+    </row>
+    <row r="7" spans="1:19" ht="14.25">
+      <c r="B7" s="162" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
+    </row>
+    <row r="10" spans="1:19" ht="12.75" thickBot="1">
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
+    </row>
+    <row r="12" spans="1:19" ht="12.75" thickBot="1">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="K13" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="L13" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="M13" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="N13" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="O13" s="128"/>
+      <c r="P13" s="128"/>
+      <c r="Q13" s="128"/>
+      <c r="R13" s="128"/>
+      <c r="S13" s="128"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="69">
+        <v>1</v>
+      </c>
+      <c r="B14" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="67"/>
+      <c r="G14" s="106" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="87"/>
+      <c r="I14" s="69">
+        <v>1</v>
+      </c>
+      <c r="J14" s="63">
+        <v>1</v>
+      </c>
+      <c r="K14" s="64">
+        <v>1</v>
+      </c>
+      <c r="L14" s="65" t="s">
+        <v>165</v>
+      </c>
+      <c r="M14" s="140">
+        <v>1440496324</v>
+      </c>
+      <c r="N14" s="67"/>
+      <c r="P14" s="127"/>
+      <c r="Q14" s="127"/>
+      <c r="R14" s="127"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="59">
+        <f>A14+1</f>
+        <v>2</v>
+      </c>
+      <c r="B15" s="138" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="141" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="67"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="59">
+        <v>2</v>
+      </c>
+      <c r="J15" s="138">
+        <v>2</v>
+      </c>
+      <c r="K15" s="141">
+        <v>1</v>
+      </c>
+      <c r="L15" s="65" t="s">
+        <v>166</v>
+      </c>
+      <c r="M15" s="140">
+        <v>1440496390</v>
+      </c>
+      <c r="N15" s="67"/>
+      <c r="P15" s="127"/>
+      <c r="Q15" s="127"/>
+      <c r="R15" s="127"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="59">
+        <f t="shared" ref="A16" si="0">A15+1</f>
+        <v>3</v>
+      </c>
+      <c r="B16" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="141" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="67"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="87"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="59">
+        <v>4</v>
+      </c>
+      <c r="B17" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="67"/>
+      <c r="G17" s="106"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="59">
+        <v>5</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="141" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="67"/>
+      <c r="G18" s="106"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="59">
+        <v>6</v>
+      </c>
+      <c r="B19" s="138" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="141" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" s="141" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="140" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" s="67"/>
+      <c r="G19" s="106"/>
+    </row>
+    <row r="20" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A20" s="70"/>
+      <c r="B20" s="131"/>
+      <c r="C20" s="132"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="134"/>
+    </row>
+    <row r="22" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="24">
+      <c r="A23" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="158" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="159"/>
+      <c r="E23" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.25">
+      <c r="A24" s="14">
+        <v>1</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="172" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="173"/>
+      <c r="E24" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="20"/>
+    </row>
+    <row r="25" spans="1:7" ht="12.95" customHeight="1">
+      <c r="A25" s="57">
+        <v>2</v>
+      </c>
+      <c r="B25" s="51"/>
+      <c r="C25" s="177"/>
+      <c r="D25" s="178"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="53"/>
+    </row>
+    <row r="26" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
+      <c r="A26" s="56">
+        <v>3</v>
+      </c>
+      <c r="B26" s="54"/>
+      <c r="C26" s="174"/>
+      <c r="D26" s="175"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="55"/>
+    </row>
+    <row r="28" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1">
+      <c r="A29" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="160" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="161"/>
+      <c r="E29" s="160" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="176"/>
+      <c r="G29" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="139" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="B31" s="139" t="s">
+        <v>168</v>
+      </c>
+      <c r="C31" s="139" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="139" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="139" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" thickBot="1">
+      <c r="A33" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="160" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="161"/>
+      <c r="E33" s="160" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="176"/>
+      <c r="G33" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8777,103 +8825,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="146" t="s">
+      <c r="C2" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="147"/>
+      <c r="D2" s="151"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="146" t="s">
+      <c r="F2" s="150" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="150"/>
+      <c r="G2" s="154"/>
     </row>
     <row r="3" spans="1:11" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="148" t="s">
+      <c r="F3" s="152" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="152"/>
+      <c r="G3" s="156"/>
     </row>
     <row r="4" spans="1:11" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="152" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="149"/>
+      <c r="D4" s="153"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="148"/>
-      <c r="G4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="156"/>
     </row>
     <row r="5" spans="1:11" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="152" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="149"/>
+      <c r="D5" s="153"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="156"/>
     </row>
     <row r="6" spans="1:11" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="152" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="149"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="152"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="156"/>
     </row>
     <row r="7" spans="1:11" ht="14.25">
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="159"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="160"/>
-      <c r="C8" s="161"/>
-      <c r="D8" s="161"/>
-      <c r="E8" s="161"/>
-      <c r="F8" s="161"/>
-      <c r="G8" s="162"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="163"/>
-      <c r="C9" s="161"/>
-      <c r="D9" s="161"/>
-      <c r="E9" s="161"/>
-      <c r="F9" s="161"/>
-      <c r="G9" s="162"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" thickBot="1">
-      <c r="B10" s="164"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="165"/>
-      <c r="G10" s="166"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9095,10 +9143,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="153" t="s">
+      <c r="C24" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="154"/>
+      <c r="D24" s="159"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -9116,10 +9164,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="167" t="s">
+      <c r="C25" s="172" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="168"/>
+      <c r="D25" s="173"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -9133,10 +9181,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="176" t="s">
+      <c r="C26" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="177"/>
+      <c r="D26" s="182"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -9155,14 +9203,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="155" t="s">
+      <c r="C29" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="156"/>
-      <c r="E29" s="155" t="s">
+      <c r="D29" s="161"/>
+      <c r="E29" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="169"/>
+      <c r="F29" s="176"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -9179,14 +9227,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="155" t="s">
+      <c r="C32" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="156"/>
-      <c r="E32" s="155" t="s">
+      <c r="D32" s="161"/>
+      <c r="E32" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="169"/>
+      <c r="F32" s="176"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -9196,14 +9244,14 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="174" t="s">
+      <c r="C33" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="175"/>
-      <c r="E33" s="176" t="s">
+      <c r="D33" s="180"/>
+      <c r="E33" s="181" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="177"/>
+      <c r="F33" s="182"/>
       <c r="G33" s="28" t="s">
         <v>49</v>
       </c>
@@ -9273,105 +9321,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="146" t="s">
+      <c r="C2" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="147"/>
+      <c r="D2" s="151"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="146" t="s">
+      <c r="F2" s="150" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="150"/>
+      <c r="G2" s="154"/>
     </row>
     <row r="3" spans="1:7" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="148" t="s">
+      <c r="F3" s="152" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="152"/>
+      <c r="G3" s="156"/>
     </row>
     <row r="4" spans="1:7" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="152" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="149"/>
+      <c r="D4" s="153"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="148"/>
-      <c r="G4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="156"/>
     </row>
     <row r="5" spans="1:7" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="152" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="149"/>
+      <c r="D5" s="153"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="156"/>
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="152" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="149"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="152"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="156"/>
     </row>
     <row r="7" spans="1:7" ht="14.25">
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="159"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="160" t="s">
+      <c r="B8" s="165" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="161"/>
-      <c r="D8" s="161"/>
-      <c r="E8" s="161"/>
-      <c r="F8" s="161"/>
-      <c r="G8" s="162"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="163"/>
-      <c r="C9" s="161"/>
-      <c r="D9" s="161"/>
-      <c r="E9" s="161"/>
-      <c r="F9" s="161"/>
-      <c r="G9" s="162"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" thickBot="1">
-      <c r="B10" s="164"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="165"/>
-      <c r="G10" s="166"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
     </row>
     <row r="12" spans="1:7" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9476,10 +9524,10 @@
       <c r="B19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="153" t="s">
+      <c r="C19" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="154"/>
+      <c r="D19" s="159"/>
       <c r="E19" s="34" t="s">
         <v>33</v>
       </c>
@@ -9497,10 +9545,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="167" t="s">
+      <c r="C20" s="172" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="168"/>
+      <c r="D20" s="173"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -9514,10 +9562,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="174" t="s">
+      <c r="C21" s="179" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="175"/>
+      <c r="D21" s="180"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
         <v>3</v>
@@ -9536,14 +9584,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="155" t="s">
+      <c r="C24" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="156"/>
-      <c r="E24" s="155" t="s">
+      <c r="D24" s="161"/>
+      <c r="E24" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="169"/>
+      <c r="F24" s="176"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -9560,14 +9608,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="155" t="s">
+      <c r="C27" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="156"/>
-      <c r="E27" s="155" t="s">
+      <c r="D27" s="161"/>
+      <c r="E27" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="169"/>
+      <c r="F27" s="176"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -9577,10 +9625,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="174"/>
-      <c r="D28" s="175"/>
-      <c r="E28" s="176"/>
-      <c r="F28" s="177"/>
+      <c r="C28" s="179"/>
+      <c r="D28" s="180"/>
+      <c r="E28" s="181"/>
+      <c r="F28" s="182"/>
       <c r="G28" s="28"/>
     </row>
   </sheetData>
@@ -9648,103 +9696,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="146" t="s">
+      <c r="C2" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="147"/>
+      <c r="D2" s="151"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="180" t="s">
+      <c r="F2" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="181"/>
+      <c r="G2" s="186"/>
     </row>
     <row r="3" spans="1:14" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="151" t="s">
+      <c r="F3" s="155" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="152"/>
+      <c r="G3" s="156"/>
     </row>
     <row r="4" spans="1:14" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="152" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="149"/>
+      <c r="D4" s="153"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="148"/>
-      <c r="G4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="156"/>
     </row>
     <row r="5" spans="1:14" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="152" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="149"/>
+      <c r="D5" s="153"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="156"/>
     </row>
     <row r="6" spans="1:14" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="152" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="149"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="152"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="156"/>
     </row>
     <row r="7" spans="1:14" ht="14.25">
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="159"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="160"/>
-      <c r="C8" s="161"/>
-      <c r="D8" s="161"/>
-      <c r="E8" s="161"/>
-      <c r="F8" s="161"/>
-      <c r="G8" s="162"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="163"/>
-      <c r="C9" s="161"/>
-      <c r="D9" s="161"/>
-      <c r="E9" s="161"/>
-      <c r="F9" s="161"/>
-      <c r="G9" s="162"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
     </row>
     <row r="10" spans="1:14" ht="12.75" thickBot="1">
-      <c r="B10" s="164"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="165"/>
-      <c r="G10" s="166"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -9960,10 +10008,10 @@
       <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="153" t="s">
+      <c r="C21" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="154"/>
+      <c r="D21" s="159"/>
       <c r="E21" s="34" t="s">
         <v>33</v>
       </c>
@@ -9987,10 +10035,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="167" t="s">
+      <c r="C22" s="172" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="168"/>
+      <c r="D22" s="173"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -10010,10 +10058,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="172" t="s">
+      <c r="C23" s="177" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="173"/>
+      <c r="D23" s="178"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -10031,10 +10079,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="174" t="s">
+      <c r="C24" s="179" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="175"/>
+      <c r="D24" s="180"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -10073,14 +10121,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="155" t="s">
+      <c r="C27" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="156"/>
-      <c r="E27" s="155" t="s">
+      <c r="D27" s="161"/>
+      <c r="E27" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="169"/>
+      <c r="F27" s="176"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -10117,14 +10165,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="155" t="s">
+      <c r="C30" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="156"/>
-      <c r="E30" s="155" t="s">
+      <c r="D30" s="161"/>
+      <c r="E30" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="169"/>
+      <c r="F30" s="176"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -10140,14 +10188,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="167" t="s">
+      <c r="C31" s="172" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="168"/>
-      <c r="E31" s="172" t="s">
+      <c r="D31" s="173"/>
+      <c r="E31" s="177" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="173"/>
+      <c r="F31" s="178"/>
       <c r="G31" s="53" t="s">
         <v>76</v>
       </c>
@@ -10163,14 +10211,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="178" t="s">
+      <c r="C32" s="183" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="179"/>
-      <c r="E32" s="176" t="s">
+      <c r="D32" s="184"/>
+      <c r="E32" s="181" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="177"/>
+      <c r="F32" s="182"/>
       <c r="G32" s="55" t="s">
         <v>52</v>
       </c>

</xml_diff>